<commit_message>
looks pretty much done
</commit_message>
<xml_diff>
--- a/misc/imgs.xlsx
+++ b/misc/imgs.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\_other\projects\nba-decision_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aelhabr\Documents\nba-decision_analysis\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$52</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -333,7 +333,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -696,11 +696,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2178,7 +2178,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C56">
+  <autoFilter ref="A1:C56" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <sortState ref="A2:D56">
       <sortCondition ref="A1:A56"/>
     </sortState>
@@ -2188,7 +2188,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>